<commit_message>
un peu de nettoyage
</commit_message>
<xml_diff>
--- a/AUT_2021/cours_2.xlsx
+++ b/AUT_2021/cours_2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meraihi_n\Desktop\ACT2035\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uqam-my.sharepoint.com/personal/meraihi_noureddine_uqam_ca/Documents/ACT2035/ACT2035/git/ACT2035/AUT_2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_4D4579C7AD784763FE10C486D2215CD62C9BDB7F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="34140" windowHeight="20480" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="departement" sheetId="3" r:id="rId1"/>
@@ -28,21 +29,30 @@
     <definedName name="employees" localSheetId="1">employee!$A$1:$K$108</definedName>
     <definedName name="employees" localSheetId="2">vlookup!$A$1:$K$108</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId9"/>
+    <pivotCache cacheId="1" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="departments" type="6" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
+  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="departments" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="C:\Users\meraihi_n\Downloads\Archive\departments.csv" decimal="," thousands=" " comma="1">
       <textFields count="4">
         <textField/>
@@ -52,7 +62,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" name="employees" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="employees" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="C:\Users\meraihi_n\Downloads\Archive\employees.csv" decimal="," thousands=" " comma="1">
       <textFields count="11">
         <textField/>
@@ -69,7 +79,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" name="employees1" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="employees1" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="C:\Users\meraihi_n\Downloads\Archive\employees.csv" decimal="," thousands=" " comma="1">
       <textFields count="11">
         <textField/>
@@ -86,7 +96,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" name="employees2" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="employees2" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="65001" sourceFile="C:\Users\meraihi_n\Downloads\Archive\employees.csv" decimal="," thousands=" " comma="1">
       <textFields count="11">
         <textField/>
@@ -1612,10 +1622,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;$&quot;_);[Red]\(#,##0.00\ &quot;$&quot;\)"/>
-    <numFmt numFmtId="44" formatCode="_ * #,##0.00_)\ &quot;$&quot;_ ;_ * \(#,##0.00\)\ &quot;$&quot;_ ;_ * &quot;-&quot;??_)\ &quot;$&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;$&quot;_);[Red]\(#,##0.00\ &quot;$&quot;\)"/>
+    <numFmt numFmtId="165" formatCode="_ * #,##0.00_)\ &quot;$&quot;_ ;_ * \(#,##0.00\)\ &quot;$&quot;_ ;_ * &quot;-&quot;??_)\ &quot;$&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -1774,7 +1784,7 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="27">
@@ -1783,7 +1793,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1792,9 +1802,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1812,18 +1822,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="44" fontId="0" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Monétaire" xfId="1" builtinId="4"/>
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Pourcentage" xfId="2" builtinId="5"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1860,7 +1870,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Profil" refreshedDate="44453.822717129631" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="29">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Profil" refreshedDate="44453.822717129631" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="29" xr:uid="{00000000-000A-0000-FFFF-FFFF03000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:D30" sheet="sumprod"/>
   </cacheSource>
@@ -2108,7 +2118,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0400-000000000000}" name="Tableau croisé dynamique1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valeurs" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="J1:K24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" showAll="0">
@@ -2249,24 +2259,27 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
     </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
   </extLst>
 </pivotTableDefinition>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="departments" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="departments" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="employees" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="employees" connectionId="2" xr16:uid="{00000000-0016-0000-0100-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="employees" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="employees" connectionId="3" xr16:uid="{00000000-0016-0000-0200-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="employees" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="employees" connectionId="4" xr16:uid="{00000000-0016-0000-0300-000003000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2531,20 +2544,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -2558,7 +2571,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>10</v>
       </c>
@@ -2572,7 +2585,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>20</v>
       </c>
@@ -2586,7 +2599,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>30</v>
       </c>
@@ -2600,7 +2613,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>40</v>
       </c>
@@ -2614,7 +2627,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>50</v>
       </c>
@@ -2628,7 +2641,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>60</v>
       </c>
@@ -2642,7 +2655,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>70</v>
       </c>
@@ -2656,7 +2669,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>80</v>
       </c>
@@ -2670,7 +2683,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>90</v>
       </c>
@@ -2684,7 +2697,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>100</v>
       </c>
@@ -2698,7 +2711,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>110</v>
       </c>
@@ -2712,7 +2725,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>120</v>
       </c>
@@ -2726,7 +2739,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>130</v>
       </c>
@@ -2740,7 +2753,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>140</v>
       </c>
@@ -2754,7 +2767,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>150</v>
       </c>
@@ -2768,7 +2781,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>160</v>
       </c>
@@ -2782,7 +2795,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>170</v>
       </c>
@@ -2796,7 +2809,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>180</v>
       </c>
@@ -2810,7 +2823,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>190</v>
       </c>
@@ -2824,7 +2837,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>200</v>
       </c>
@@ -2838,7 +2851,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>210</v>
       </c>
@@ -2852,7 +2865,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>220</v>
       </c>
@@ -2866,7 +2879,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>230</v>
       </c>
@@ -2880,7 +2893,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>240</v>
       </c>
@@ -2894,7 +2907,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>250</v>
       </c>
@@ -2908,7 +2921,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>260</v>
       </c>
@@ -2922,7 +2935,7 @@
         <v>1700</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>270</v>
       </c>
@@ -2942,28 +2955,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K108"/>
   <sheetViews>
     <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2998,7 +3011,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>100</v>
       </c>
@@ -3033,7 +3046,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>101</v>
       </c>
@@ -3068,7 +3081,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>102</v>
       </c>
@@ -3103,7 +3116,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>103</v>
       </c>
@@ -3138,7 +3151,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>104</v>
       </c>
@@ -3173,7 +3186,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>105</v>
       </c>
@@ -3208,7 +3221,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>106</v>
       </c>
@@ -3243,7 +3256,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>107</v>
       </c>
@@ -3278,7 +3291,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>108</v>
       </c>
@@ -3313,7 +3326,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>109</v>
       </c>
@@ -3348,7 +3361,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>110</v>
       </c>
@@ -3383,7 +3396,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>111</v>
       </c>
@@ -3418,7 +3431,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>112</v>
       </c>
@@ -3453,7 +3466,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>113</v>
       </c>
@@ -3488,7 +3501,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>114</v>
       </c>
@@ -3523,7 +3536,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>115</v>
       </c>
@@ -3558,7 +3571,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>116</v>
       </c>
@@ -3593,7 +3606,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>117</v>
       </c>
@@ -3628,7 +3641,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>118</v>
       </c>
@@ -3663,7 +3676,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>119</v>
       </c>
@@ -3698,7 +3711,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>120</v>
       </c>
@@ -3733,7 +3746,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>121</v>
       </c>
@@ -3768,7 +3781,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>122</v>
       </c>
@@ -3803,7 +3816,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>123</v>
       </c>
@@ -3838,7 +3851,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>124</v>
       </c>
@@ -3873,7 +3886,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>125</v>
       </c>
@@ -3908,7 +3921,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>126</v>
       </c>
@@ -3943,7 +3956,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>127</v>
       </c>
@@ -3978,7 +3991,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>128</v>
       </c>
@@ -4013,7 +4026,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>129</v>
       </c>
@@ -4048,7 +4061,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>130</v>
       </c>
@@ -4083,7 +4096,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>131</v>
       </c>
@@ -4118,7 +4131,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>132</v>
       </c>
@@ -4153,7 +4166,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>133</v>
       </c>
@@ -4188,7 +4201,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>134</v>
       </c>
@@ -4223,7 +4236,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>135</v>
       </c>
@@ -4258,7 +4271,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>136</v>
       </c>
@@ -4293,7 +4306,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>137</v>
       </c>
@@ -4328,7 +4341,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>138</v>
       </c>
@@ -4363,7 +4376,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>139</v>
       </c>
@@ -4398,7 +4411,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>140</v>
       </c>
@@ -4433,7 +4446,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>141</v>
       </c>
@@ -4468,7 +4481,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>142</v>
       </c>
@@ -4503,7 +4516,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>143</v>
       </c>
@@ -4538,7 +4551,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>144</v>
       </c>
@@ -4573,7 +4586,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>145</v>
       </c>
@@ -4608,7 +4621,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>146</v>
       </c>
@@ -4643,7 +4656,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>147</v>
       </c>
@@ -4678,7 +4691,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>148</v>
       </c>
@@ -4713,7 +4726,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>149</v>
       </c>
@@ -4748,7 +4761,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>150</v>
       </c>
@@ -4783,7 +4796,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>151</v>
       </c>
@@ -4818,7 +4831,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>152</v>
       </c>
@@ -4853,7 +4866,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>153</v>
       </c>
@@ -4888,7 +4901,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>154</v>
       </c>
@@ -4923,7 +4936,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>155</v>
       </c>
@@ -4958,7 +4971,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>156</v>
       </c>
@@ -4993,7 +5006,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>157</v>
       </c>
@@ -5028,7 +5041,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>158</v>
       </c>
@@ -5063,7 +5076,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>159</v>
       </c>
@@ -5098,7 +5111,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>160</v>
       </c>
@@ -5133,7 +5146,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>161</v>
       </c>
@@ -5168,7 +5181,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>162</v>
       </c>
@@ -5203,7 +5216,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>163</v>
       </c>
@@ -5238,7 +5251,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>164</v>
       </c>
@@ -5273,7 +5286,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>165</v>
       </c>
@@ -5308,7 +5321,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>166</v>
       </c>
@@ -5343,7 +5356,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>167</v>
       </c>
@@ -5378,7 +5391,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>168</v>
       </c>
@@ -5413,7 +5426,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>169</v>
       </c>
@@ -5448,7 +5461,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>170</v>
       </c>
@@ -5483,7 +5496,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>171</v>
       </c>
@@ -5518,7 +5531,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>172</v>
       </c>
@@ -5553,7 +5566,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>173</v>
       </c>
@@ -5588,7 +5601,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>174</v>
       </c>
@@ -5623,7 +5636,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>175</v>
       </c>
@@ -5658,7 +5671,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>176</v>
       </c>
@@ -5693,7 +5706,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>177</v>
       </c>
@@ -5728,7 +5741,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>178</v>
       </c>
@@ -5763,7 +5776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>179</v>
       </c>
@@ -5798,7 +5811,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>180</v>
       </c>
@@ -5833,7 +5846,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>181</v>
       </c>
@@ -5868,7 +5881,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>182</v>
       </c>
@@ -5903,7 +5916,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>183</v>
       </c>
@@ -5938,7 +5951,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>184</v>
       </c>
@@ -5973,7 +5986,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>185</v>
       </c>
@@ -6008,7 +6021,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>186</v>
       </c>
@@ -6043,7 +6056,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>187</v>
       </c>
@@ -6078,7 +6091,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>188</v>
       </c>
@@ -6113,7 +6126,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>189</v>
       </c>
@@ -6148,7 +6161,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>190</v>
       </c>
@@ -6183,7 +6196,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>191</v>
       </c>
@@ -6218,7 +6231,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>192</v>
       </c>
@@ -6253,7 +6266,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>193</v>
       </c>
@@ -6288,7 +6301,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>194</v>
       </c>
@@ -6323,7 +6336,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>195</v>
       </c>
@@ -6358,7 +6371,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>196</v>
       </c>
@@ -6393,7 +6406,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>197</v>
       </c>
@@ -6428,7 +6441,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>198</v>
       </c>
@@ -6463,7 +6476,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>199</v>
       </c>
@@ -6498,7 +6511,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>200</v>
       </c>
@@ -6533,7 +6546,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>201</v>
       </c>
@@ -6568,7 +6581,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>202</v>
       </c>
@@ -6603,7 +6616,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>203</v>
       </c>
@@ -6638,7 +6651,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>204</v>
       </c>
@@ -6673,7 +6686,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>205</v>
       </c>
@@ -6708,7 +6721,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>206</v>
       </c>
@@ -6749,22 +6762,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N108"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="10" width="11.42578125" style="2"/>
-    <col min="11" max="11" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.7109375" style="4" customWidth="1"/>
-    <col min="13" max="13" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="10" width="11.5" style="2"/>
+    <col min="11" max="11" width="15.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.6640625" style="4" customWidth="1"/>
+    <col min="13" max="13" width="28.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6808,7 +6821,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>100</v>
       </c>
@@ -6855,7 +6868,7 @@
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>101</v>
       </c>
@@ -6902,7 +6915,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>102</v>
       </c>
@@ -6949,7 +6962,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>103</v>
       </c>
@@ -6996,7 +7009,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>104</v>
       </c>
@@ -7043,7 +7056,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>105</v>
       </c>
@@ -7090,7 +7103,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>106</v>
       </c>
@@ -7137,7 +7150,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>107</v>
       </c>
@@ -7184,7 +7197,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>108</v>
       </c>
@@ -7231,7 +7244,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>109</v>
       </c>
@@ -7278,7 +7291,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>110</v>
       </c>
@@ -7325,7 +7338,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>111</v>
       </c>
@@ -7372,7 +7385,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>112</v>
       </c>
@@ -7419,7 +7432,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>113</v>
       </c>
@@ -7466,7 +7479,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>114</v>
       </c>
@@ -7513,7 +7526,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>115</v>
       </c>
@@ -7560,7 +7573,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>116</v>
       </c>
@@ -7607,7 +7620,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>117</v>
       </c>
@@ -7654,7 +7667,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>118</v>
       </c>
@@ -7701,7 +7714,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>119</v>
       </c>
@@ -7748,7 +7761,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>120</v>
       </c>
@@ -7795,7 +7808,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>121</v>
       </c>
@@ -7842,7 +7855,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>122</v>
       </c>
@@ -7889,7 +7902,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>123</v>
       </c>
@@ -7936,7 +7949,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>124</v>
       </c>
@@ -7983,7 +7996,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>125</v>
       </c>
@@ -8030,7 +8043,7 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>126</v>
       </c>
@@ -8077,7 +8090,7 @@
         <v/>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>127</v>
       </c>
@@ -8124,7 +8137,7 @@
         <v/>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>128</v>
       </c>
@@ -8171,7 +8184,7 @@
         <v/>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>129</v>
       </c>
@@ -8218,7 +8231,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>130</v>
       </c>
@@ -8265,7 +8278,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>131</v>
       </c>
@@ -8312,7 +8325,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>132</v>
       </c>
@@ -8359,7 +8372,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>133</v>
       </c>
@@ -8406,7 +8419,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>134</v>
       </c>
@@ -8453,7 +8466,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>135</v>
       </c>
@@ -8500,7 +8513,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>136</v>
       </c>
@@ -8547,7 +8560,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>137</v>
       </c>
@@ -8594,7 +8607,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>138</v>
       </c>
@@ -8641,7 +8654,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>139</v>
       </c>
@@ -8688,7 +8701,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>140</v>
       </c>
@@ -8735,7 +8748,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>141</v>
       </c>
@@ -8782,7 +8795,7 @@
         <v/>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>142</v>
       </c>
@@ -8829,7 +8842,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>143</v>
       </c>
@@ -8876,7 +8889,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>144</v>
       </c>
@@ -8923,7 +8936,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>145</v>
       </c>
@@ -8970,7 +8983,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>146</v>
       </c>
@@ -9017,7 +9030,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>147</v>
       </c>
@@ -9064,7 +9077,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>148</v>
       </c>
@@ -9111,7 +9124,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>149</v>
       </c>
@@ -9158,7 +9171,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>150</v>
       </c>
@@ -9205,7 +9218,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>151</v>
       </c>
@@ -9252,7 +9265,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>152</v>
       </c>
@@ -9299,7 +9312,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>153</v>
       </c>
@@ -9346,7 +9359,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>154</v>
       </c>
@@ -9393,7 +9406,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>155</v>
       </c>
@@ -9440,7 +9453,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>156</v>
       </c>
@@ -9487,7 +9500,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>157</v>
       </c>
@@ -9534,7 +9547,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A60" s="2">
         <v>158</v>
       </c>
@@ -9581,7 +9594,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>159</v>
       </c>
@@ -9628,7 +9641,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
         <v>160</v>
       </c>
@@ -9675,7 +9688,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
         <v>161</v>
       </c>
@@ -9722,7 +9735,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
         <v>162</v>
       </c>
@@ -9769,7 +9782,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>163</v>
       </c>
@@ -9816,7 +9829,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>164</v>
       </c>
@@ -9863,7 +9876,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>165</v>
       </c>
@@ -9910,7 +9923,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>166</v>
       </c>
@@ -9957,7 +9970,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>167</v>
       </c>
@@ -10004,7 +10017,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>168</v>
       </c>
@@ -10051,7 +10064,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>169</v>
       </c>
@@ -10098,7 +10111,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>170</v>
       </c>
@@ -10145,7 +10158,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>171</v>
       </c>
@@ -10192,7 +10205,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>172</v>
       </c>
@@ -10239,7 +10252,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>173</v>
       </c>
@@ -10286,7 +10299,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>174</v>
       </c>
@@ -10333,7 +10346,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>175</v>
       </c>
@@ -10380,7 +10393,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>176</v>
       </c>
@@ -10427,7 +10440,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>177</v>
       </c>
@@ -10474,7 +10487,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>178</v>
       </c>
@@ -10521,7 +10534,7 @@
         <v>#N/A</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>179</v>
       </c>
@@ -10568,7 +10581,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A82" s="2">
         <v>180</v>
       </c>
@@ -10615,7 +10628,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A83" s="2">
         <v>181</v>
       </c>
@@ -10662,7 +10675,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A84" s="2">
         <v>182</v>
       </c>
@@ -10709,7 +10722,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A85" s="2">
         <v>183</v>
       </c>
@@ -10756,7 +10769,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A86" s="2">
         <v>184</v>
       </c>
@@ -10803,7 +10816,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A87" s="2">
         <v>185</v>
       </c>
@@ -10850,7 +10863,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A88" s="2">
         <v>186</v>
       </c>
@@ -10897,7 +10910,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A89" s="2">
         <v>187</v>
       </c>
@@ -10944,7 +10957,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A90" s="2">
         <v>188</v>
       </c>
@@ -10991,7 +11004,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A91" s="2">
         <v>189</v>
       </c>
@@ -11038,7 +11051,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A92" s="2">
         <v>190</v>
       </c>
@@ -11085,7 +11098,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A93" s="2">
         <v>191</v>
       </c>
@@ -11132,7 +11145,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A94" s="2">
         <v>192</v>
       </c>
@@ -11179,7 +11192,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A95" s="2">
         <v>193</v>
       </c>
@@ -11226,7 +11239,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A96" s="2">
         <v>194</v>
       </c>
@@ -11273,7 +11286,7 @@
         <v/>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A97" s="2">
         <v>195</v>
       </c>
@@ -11320,7 +11333,7 @@
         <v/>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>196</v>
       </c>
@@ -11367,7 +11380,7 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A99" s="2">
         <v>197</v>
       </c>
@@ -11414,7 +11427,7 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A100" s="2">
         <v>198</v>
       </c>
@@ -11461,7 +11474,7 @@
         <v/>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A101" s="2">
         <v>199</v>
       </c>
@@ -11508,7 +11521,7 @@
         <v/>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" s="2">
         <v>200</v>
       </c>
@@ -11555,7 +11568,7 @@
         <v/>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" s="2">
         <v>201</v>
       </c>
@@ -11602,7 +11615,7 @@
         <v/>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" s="2">
         <v>202</v>
       </c>
@@ -11649,7 +11662,7 @@
         <v/>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" s="2">
         <v>203</v>
       </c>
@@ -11696,7 +11709,7 @@
         <v/>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" s="2">
         <v>204</v>
       </c>
@@ -11743,7 +11756,7 @@
         <v/>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>205</v>
       </c>
@@ -11790,7 +11803,7 @@
         <v/>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108" s="2">
         <v>206</v>
       </c>
@@ -11838,36 +11851,36 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:N108"/>
+  <autoFilter ref="A1:N108" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:P108"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.42578125" style="6"/>
-    <col min="15" max="15" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" style="6"/>
+    <col min="15" max="15" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -11908,7 +11921,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>100</v>
       </c>
@@ -11953,7 +11966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>101</v>
       </c>
@@ -12001,7 +12014,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>102</v>
       </c>
@@ -12049,7 +12062,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>103</v>
       </c>
@@ -12097,7 +12110,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>104</v>
       </c>
@@ -12136,7 +12149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>105</v>
       </c>
@@ -12175,7 +12188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>106</v>
       </c>
@@ -12214,7 +12227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>107</v>
       </c>
@@ -12253,7 +12266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>108</v>
       </c>
@@ -12292,7 +12305,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>109</v>
       </c>
@@ -12331,7 +12344,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>110</v>
       </c>
@@ -12370,7 +12383,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>111</v>
       </c>
@@ -12409,7 +12422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>112</v>
       </c>
@@ -12448,7 +12461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>113</v>
       </c>
@@ -12487,7 +12500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>114</v>
       </c>
@@ -12526,7 +12539,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>115</v>
       </c>
@@ -12565,7 +12578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>116</v>
       </c>
@@ -12604,7 +12617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>117</v>
       </c>
@@ -12643,7 +12656,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>118</v>
       </c>
@@ -12682,7 +12695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>119</v>
       </c>
@@ -12721,7 +12734,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>120</v>
       </c>
@@ -12760,7 +12773,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>121</v>
       </c>
@@ -12799,7 +12812,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>122</v>
       </c>
@@ -12838,7 +12851,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>123</v>
       </c>
@@ -12877,7 +12890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>124</v>
       </c>
@@ -12916,7 +12929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>125</v>
       </c>
@@ -12955,7 +12968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>126</v>
       </c>
@@ -12994,7 +13007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>127</v>
       </c>
@@ -13033,7 +13046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>128</v>
       </c>
@@ -13072,7 +13085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>129</v>
       </c>
@@ -13111,7 +13124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>130</v>
       </c>
@@ -13150,7 +13163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>131</v>
       </c>
@@ -13189,7 +13202,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>132</v>
       </c>
@@ -13228,7 +13241,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>133</v>
       </c>
@@ -13267,7 +13280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>134</v>
       </c>
@@ -13306,7 +13319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>135</v>
       </c>
@@ -13345,7 +13358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>136</v>
       </c>
@@ -13384,7 +13397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>137</v>
       </c>
@@ -13423,7 +13436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>138</v>
       </c>
@@ -13462,7 +13475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>139</v>
       </c>
@@ -13501,7 +13514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>140</v>
       </c>
@@ -13540,7 +13553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>141</v>
       </c>
@@ -13579,7 +13592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>142</v>
       </c>
@@ -13618,7 +13631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>143</v>
       </c>
@@ -13657,7 +13670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>144</v>
       </c>
@@ -13696,7 +13709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>145</v>
       </c>
@@ -13735,7 +13748,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>146</v>
       </c>
@@ -13774,7 +13787,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>147</v>
       </c>
@@ -13813,7 +13826,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>148</v>
       </c>
@@ -13852,7 +13865,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>149</v>
       </c>
@@ -13891,7 +13904,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>150</v>
       </c>
@@ -13930,7 +13943,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>151</v>
       </c>
@@ -13969,7 +13982,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>152</v>
       </c>
@@ -14008,7 +14021,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>153</v>
       </c>
@@ -14047,7 +14060,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>154</v>
       </c>
@@ -14086,7 +14099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>155</v>
       </c>
@@ -14125,7 +14138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>156</v>
       </c>
@@ -14164,7 +14177,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>157</v>
       </c>
@@ -14203,7 +14216,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>158</v>
       </c>
@@ -14242,7 +14255,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>159</v>
       </c>
@@ -14281,7 +14294,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>160</v>
       </c>
@@ -14320,7 +14333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>161</v>
       </c>
@@ -14359,7 +14372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>162</v>
       </c>
@@ -14398,7 +14411,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>163</v>
       </c>
@@ -14437,7 +14450,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>164</v>
       </c>
@@ -14476,7 +14489,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>165</v>
       </c>
@@ -14515,7 +14528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>166</v>
       </c>
@@ -14554,7 +14567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>167</v>
       </c>
@@ -14593,7 +14606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>168</v>
       </c>
@@ -14632,7 +14645,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>169</v>
       </c>
@@ -14671,7 +14684,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>170</v>
       </c>
@@ -14710,7 +14723,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>171</v>
       </c>
@@ -14749,7 +14762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>172</v>
       </c>
@@ -14788,7 +14801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>173</v>
       </c>
@@ -14827,7 +14840,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>174</v>
       </c>
@@ -14866,7 +14879,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>175</v>
       </c>
@@ -14905,7 +14918,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>176</v>
       </c>
@@ -14944,7 +14957,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>177</v>
       </c>
@@ -14983,7 +14996,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>178</v>
       </c>
@@ -15022,7 +15035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>179</v>
       </c>
@@ -15061,7 +15074,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>180</v>
       </c>
@@ -15100,7 +15113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>181</v>
       </c>
@@ -15139,7 +15152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>182</v>
       </c>
@@ -15178,7 +15191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>183</v>
       </c>
@@ -15217,7 +15230,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>184</v>
       </c>
@@ -15256,7 +15269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>185</v>
       </c>
@@ -15295,7 +15308,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>186</v>
       </c>
@@ -15334,7 +15347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>187</v>
       </c>
@@ -15373,7 +15386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>188</v>
       </c>
@@ -15412,7 +15425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>189</v>
       </c>
@@ -15451,7 +15464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>190</v>
       </c>
@@ -15490,7 +15503,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>191</v>
       </c>
@@ -15529,7 +15542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>192</v>
       </c>
@@ -15568,7 +15581,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>193</v>
       </c>
@@ -15607,7 +15620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>194</v>
       </c>
@@ -15646,7 +15659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>195</v>
       </c>
@@ -15685,7 +15698,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>196</v>
       </c>
@@ -15724,7 +15737,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>197</v>
       </c>
@@ -15763,7 +15776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>198</v>
       </c>
@@ -15802,7 +15815,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>199</v>
       </c>
@@ -15841,7 +15854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>200</v>
       </c>
@@ -15880,7 +15893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>201</v>
       </c>
@@ -15919,7 +15932,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>202</v>
       </c>
@@ -15958,7 +15971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>203</v>
       </c>
@@ -15997,7 +16010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>204</v>
       </c>
@@ -16036,7 +16049,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>205</v>
       </c>
@@ -16075,7 +16088,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>206</v>
       </c>
@@ -16121,25 +16134,25 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="4" width="11.42578125" style="14"/>
-    <col min="6" max="9" width="1.5703125" customWidth="1"/>
+    <col min="2" max="4" width="11.5" style="14"/>
+    <col min="6" max="9" width="1.5" customWidth="1"/>
     <col min="10" max="10" width="21" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" customWidth="1"/>
-    <col min="12" max="27" width="23.85546875" customWidth="1"/>
-    <col min="28" max="28" width="12.5703125" customWidth="1"/>
-    <col min="29" max="29" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5" customWidth="1"/>
+    <col min="12" max="27" width="23.83203125" customWidth="1"/>
+    <col min="28" max="28" width="12.5" customWidth="1"/>
+    <col min="29" max="29" width="12.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>479</v>
       </c>
@@ -16159,7 +16172,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -16189,7 +16202,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="17" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -16220,7 +16233,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -16244,7 +16257,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -16268,7 +16281,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -16292,7 +16305,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -16316,7 +16329,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -16340,7 +16353,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>42</v>
       </c>
@@ -16364,7 +16377,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>46</v>
       </c>
@@ -16388,7 +16401,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>51</v>
       </c>
@@ -16412,7 +16425,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -16436,7 +16449,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>60</v>
       </c>
@@ -16460,7 +16473,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>64</v>
       </c>
@@ -16484,7 +16497,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>68</v>
       </c>
@@ -16508,7 +16521,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>72</v>
       </c>
@@ -16532,7 +16545,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -16556,7 +16569,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>81</v>
       </c>
@@ -16580,7 +16593,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>85</v>
       </c>
@@ -16604,7 +16617,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>60</v>
       </c>
@@ -16628,7 +16641,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>93</v>
       </c>
@@ -16652,7 +16665,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>97</v>
       </c>
@@ -16676,7 +16689,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>114</v>
       </c>
@@ -16700,7 +16713,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>106</v>
       </c>
@@ -16721,7 +16734,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>110</v>
       </c>
@@ -16736,7 +16749,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>114</v>
       </c>
@@ -16751,7 +16764,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>118</v>
       </c>
@@ -16766,7 +16779,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>123</v>
       </c>
@@ -16781,7 +16794,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>118</v>
       </c>
@@ -16796,7 +16809,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>11</v>
       </c>
@@ -16819,7 +16832,7 @@
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M3" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>$Q$2:$Q$23</formula1>
     </dataValidation>
   </dataValidations>
@@ -16828,16 +16841,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B1" s="19">
         <v>1</v>
       </c>
@@ -16866,7 +16879,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="19">
         <v>1</v>
       </c>
@@ -16875,42 +16888,42 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="19">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="19">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="19">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="19">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="19">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="19">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="19">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="19">
         <v>9</v>
       </c>
@@ -16921,21 +16934,21 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>488</v>
       </c>
@@ -16961,7 +16974,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>489</v>
       </c>
@@ -16987,7 +17000,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>490</v>
       </c>
@@ -17013,7 +17026,7 @@
         <v>-7586.7958220383725</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>491</v>
       </c>
@@ -17039,7 +17052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>492</v>
       </c>
@@ -17078,24 +17091,24 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="15" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="15" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>495</v>
       </c>
@@ -17103,7 +17116,7 @@
         <v>-50000</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>488</v>
       </c>
@@ -17111,7 +17124,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>496</v>
       </c>
@@ -17142,7 +17155,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>497</v>
       </c>
@@ -17173,7 +17186,7 @@
         <v>8845.1963623431293</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>498</v>
       </c>
@@ -17181,10 +17194,10 @@
         <v>40000</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B6" s="5"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>499</v>
       </c>
@@ -17197,12 +17210,12 @@
         <v>11352.660249736349</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E8" s="24">
         <v>-50000</v>
       </c>
       <c r="F8" s="5">
-        <f t="dataTable" ref="F8:F14" dt2D="0" dtr="0" r1="B1"/>
+        <f t="dataTable" ref="F8:F14" dt2D="0" dtr="0" r1="B1" ca="1"/>
         <v>11352.660249736349</v>
       </c>
       <c r="I8" s="26">
@@ -17233,7 +17246,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E9" s="24">
         <f>E8+5000</f>
         <v>-45000</v>
@@ -17245,7 +17258,7 @@
         <v>-50000</v>
       </c>
       <c r="J9" s="5">
-        <f t="dataTable" ref="J9:O15" dt2D="1" dtr="1" r1="B2" r2="B1" ca="1"/>
+        <f t="dataTable" ref="J9:O15" dt2D="1" dtr="1" r1="B2" r2="B1"/>
         <v>15449.101193619266</v>
       </c>
       <c r="K9" s="5">
@@ -17264,7 +17277,7 @@
         <v>8845.1963623431293</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E10" s="24">
         <f t="shared" ref="E10:E13" si="2">E9+5000</f>
         <v>-40000</v>
@@ -17295,7 +17308,7 @@
         <v>13845.196362343129</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E11" s="24">
         <f t="shared" si="2"/>
         <v>-35000</v>
@@ -17326,7 +17339,7 @@
         <v>18845.196362343129</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E12" s="24">
         <f t="shared" si="2"/>
         <v>-30000</v>
@@ -17357,7 +17370,7 @@
         <v>23845.196362343129</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E13" s="24">
         <f t="shared" si="2"/>
         <v>-25000</v>
@@ -17388,7 +17401,7 @@
         <v>28845.196362343129</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="E14" s="24">
         <f>E13+5000</f>
         <v>-20000</v>
@@ -17419,7 +17432,7 @@
         <v>33845.196362343129</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="I15" s="24">
         <f>I14+5000</f>
         <v>-20000</v>

</xml_diff>